<commit_message>
Added test method for Login Forgot Email
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Myfolder\workspace\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forgot email-web\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7156321-6E28-452D-97A9-55AB70EB47BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50CBF38-E133-42FE-84EB-84014E9E0978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10500" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="95">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -515,6 +515,20 @@
 -pauthyHeading,
 -psecurityKey,
 -pmessage</t>
+  </si>
+  <si>
+    <t>Forgot email with go back option</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.LoginTest,
+testForgotEmailwithBackActions,
+-ploginHeading,
+-pForgotHeading,
+-pphoneNumber,
+-pfirstName,
+-plastName,
+-perrMessage,
+-pcolour</t>
   </si>
 </sst>
 </file>
@@ -909,30 +923,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" customWidth="1"/>
-    <col min="8" max="8" width="51.6640625" customWidth="1"/>
-    <col min="9" max="9" width="44.5546875" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.08984375" customWidth="1"/>
+    <col min="7" max="7" width="31.08984375" customWidth="1"/>
+    <col min="8" max="8" width="51.6328125" customWidth="1"/>
+    <col min="9" max="9" width="44.54296875" customWidth="1"/>
+    <col min="10" max="10" width="25.6328125" customWidth="1"/>
+    <col min="11" max="11" width="25.36328125" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.36328125" customWidth="1"/>
+    <col min="14" max="14" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -962,7 +976,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -989,7 +1003,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1029,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1067,7 +1081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1093,9 +1107,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>43</v>
@@ -1116,12 +1130,12 @@
         <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>43</v>
@@ -1136,18 +1150,18 @@
         <v>13</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>43</v>
@@ -1162,47 +1176,44 @@
         <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>43</v>
@@ -1226,12 +1237,12 @@
         <v>29</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>43</v>
@@ -1255,12 +1266,12 @@
         <v>29</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>43</v>
@@ -1284,12 +1295,12 @@
         <v>29</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>43</v>
@@ -1313,12 +1324,12 @@
         <v>29</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>43</v>
@@ -1342,12 +1353,12 @@
         <v>29</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>43</v>
@@ -1361,8 +1372,8 @@
       <c r="E16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>41</v>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>28</v>
@@ -1371,41 +1382,41 @@
         <v>29</v>
       </c>
       <c r="I16" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="18" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>43</v>
@@ -1429,12 +1440,12 @@
         <v>29</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>43</v>
@@ -1458,12 +1469,12 @@
         <v>29</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>43</v>
@@ -1487,12 +1498,12 @@
         <v>29</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>43</v>
@@ -1515,13 +1526,13 @@
       <c r="H21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I21" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>43</v>
@@ -1544,13 +1555,13 @@
       <c r="H22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I22" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>43</v>
@@ -1573,13 +1584,13 @@
       <c r="H23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I23" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>43</v>
@@ -1602,13 +1613,13 @@
       <c r="H24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I24" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>43</v>
@@ -1631,13 +1642,13 @@
       <c r="H25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I25" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>43</v>
@@ -1660,13 +1671,13 @@
       <c r="H26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I26" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>43</v>
@@ -1690,12 +1701,12 @@
         <v>29</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>43</v>
@@ -1719,12 +1730,12 @@
         <v>29</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>43</v>
@@ -1748,12 +1759,12 @@
         <v>29</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>43</v>
@@ -1777,12 +1788,12 @@
         <v>29</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>43</v>
@@ -1805,57 +1816,57 @@
       <c r="H31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="8" t="s">
+      <c r="D33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>28</v>
@@ -1864,35 +1875,64 @@
         <v>29</v>
       </c>
       <c r="I33" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="232" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+    <row r="35" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I34" s="10" t="s">
+      <c r="H35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1911,7 +1951,7 @@
           <x14:formula1>
             <xm:f>lists!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B34</xm:sqref>
+          <xm:sqref>B1:B35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1927,12 +1967,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -1940,7 +1980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1948,7 +1988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Added field validation in Forgot Email
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ideyalabs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\web (05-01-2022)[2]\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EAE872-7AF7-4901-B11A-37281300B944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27CF0DC-2C1D-4BCB-BA98-2D105E7DC81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="97">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -250,24 +250,10 @@
 -plastName</t>
   </si>
   <si>
-    <t>Verify Available Balance in Token Account</t>
-  </si>
-  <si>
     <t>testdata.xlsx,TokenAccount-Customer</t>
   </si>
   <si>
     <t>Token Account</t>
-  </si>
-  <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testAvailableBalance</t>
-  </si>
-  <si>
-    <t>Verify PayAndRequestTokens in Token Account</t>
-  </si>
-  <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testPayAndRequestTokens</t>
   </si>
   <si>
     <t>Verify BuyTokens in Token Account</t>
@@ -536,6 +522,42 @@
   <si>
     <t>coyni.customer.tests.CustomerProfileTest,
 testNotificationsDelete</t>
+  </si>
+  <si>
+    <t>Forgot email with field validation</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.LoginTest,
+testForgotEmailWithValidatePhoneNumber,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber</t>
+  </si>
+  <si>
+    <t>Forgot email with field validation with first and last name</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.LoginTest,
+testForgotEmailWithValidateFirstAndLastName,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber,
+-pfirstName,
+-plastName</t>
+  </si>
+  <si>
+    <t>Forgot email with resend option</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.LoginTest,
+testForgotEmailWithResendOption,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber,
+-pfirstName,
+-plastName,
+-PverificationHeading,
+-PverifyPhoneNumber</t>
   </si>
 </sst>
 </file>
@@ -975,25 +997,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.08984375" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.08984375" customWidth="1"/>
-    <col min="7" max="7" width="31.08984375" customWidth="1"/>
-    <col min="8" max="8" width="51.6328125" customWidth="1"/>
-    <col min="9" max="9" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
+    <col min="8" max="8" width="51.6640625" customWidth="1"/>
+    <col min="9" max="9" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="137" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="136.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1071,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="163.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1098,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="103.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1125,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1130,7 +1152,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="136.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -1157,7 +1179,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="104.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -1184,7 +1206,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>17</v>
@@ -1204,14 +1226,14 @@
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -1219,7 +1241,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>17</v>
@@ -1231,14 +1253,14 @@
         <v>34</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1246,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>17</v>
@@ -1255,17 +1277,17 @@
         <v>13</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1295,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>17</v>
@@ -1285,14 +1307,14 @@
         <v>34</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1300,7 +1322,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>17</v>
@@ -1312,167 +1334,161 @@
         <v>13</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>17</v>
@@ -1484,24 +1500,24 @@
         <v>13</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>17</v>
@@ -1513,54 +1529,53 @@
         <v>13</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>17</v>
@@ -1572,25 +1587,25 @@
         <v>13</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>17</v>
@@ -1602,25 +1617,25 @@
         <v>13</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>17</v>
@@ -1632,83 +1647,84 @@
         <v>13</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="2">
+    <row r="24" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>17</v>
@@ -1720,24 +1736,24 @@
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
-        <v>69</v>
+      <c r="I26" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>17</v>
@@ -1745,28 +1761,28 @@
       <c r="E27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>86</v>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="I27" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>17</v>
@@ -1774,57 +1790,57 @@
       <c r="E28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
+      <c r="F28" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>15</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="203" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="18" t="s">
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>15</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>17</v>
@@ -1836,82 +1852,82 @@
         <v>13</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="18" t="s">
         <v>15</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" t="s">
-        <v>63</v>
+      <c r="C31" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>15</v>
       </c>
       <c r="I31" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="232" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="18" t="s">
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="16" t="s">
         <v>15</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>17</v>
@@ -1920,16 +1936,45 @@
         <v>13</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>15</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1964,12 +2009,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1977,7 +2022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1985,9 +2030,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regression fixes for Customer and admin
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpace-08-01-2022\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Code-push\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401B59AD-C6D7-488F-A684-8B9AF61A0AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFE43CC-7B85-4E40-B929-21F448F603F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -1224,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1272,9 +1272,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1298,12 +1295,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1633,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,9 +1696,9 @@
       <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="137.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1734,9 +1725,9 @@
       <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="163.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1763,9 +1754,9 @@
       <c r="H4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1792,9 +1783,9 @@
       <c r="H5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1821,9 +1812,9 @@
       <c r="H6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1850,9 +1841,9 @@
       <c r="H7" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1879,9 +1870,9 @@
       <c r="H8" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1908,9 +1899,9 @@
       <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1937,9 +1928,9 @@
       <c r="H10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1966,9 +1957,9 @@
       <c r="H11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
@@ -1992,12 +1983,12 @@
       <c r="G12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -2021,12 +2012,12 @@
       <c r="G13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
@@ -2050,12 +2041,12 @@
       <c r="G14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -2079,12 +2070,12 @@
       <c r="G15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -2108,12 +2099,12 @@
       <c r="G16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -2137,12 +2128,12 @@
       <c r="G17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -2166,12 +2157,12 @@
       <c r="G18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
@@ -2195,14 +2186,14 @@
       <c r="G19" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -2226,14 +2217,14 @@
       <c r="G20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="22" t="s">
+      <c r="H20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
@@ -2257,14 +2248,14 @@
       <c r="G21" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="22" t="s">
+      <c r="H21" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -2288,14 +2279,14 @@
       <c r="G22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" s="22" t="s">
+      <c r="H22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
@@ -2319,14 +2310,14 @@
       <c r="G23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="18" t="s">
+      <c r="H23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
@@ -2350,14 +2341,14 @@
       <c r="G24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="18" t="s">
+      <c r="H24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -2381,14 +2372,14 @@
       <c r="G25" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="22" t="s">
+      <c r="H25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -2412,14 +2403,14 @@
       <c r="G26" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="22" t="s">
+      <c r="H26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -2443,14 +2434,14 @@
       <c r="G27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" s="22" t="s">
+      <c r="H27" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="139.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -2474,14 +2465,14 @@
       <c r="G28" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" s="18" t="s">
+      <c r="H28" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -2508,11 +2499,11 @@
       <c r="H29" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
     </row>
     <row r="30" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -2539,11 +2530,11 @@
       <c r="H30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -2573,8 +2564,8 @@
       <c r="I31" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
@@ -2601,11 +2592,11 @@
       <c r="H32" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
@@ -2632,11 +2623,11 @@
       <c r="H33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="23" t="s">
+      <c r="I33" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -2663,11 +2654,11 @@
       <c r="H34" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I34" s="23" t="s">
+      <c r="I34" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2694,11 +2685,11 @@
       <c r="H35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -2725,11 +2716,11 @@
       <c r="H36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
     </row>
     <row r="37" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2756,11 +2747,11 @@
       <c r="H37" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I37" s="23" t="s">
+      <c r="I37" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
     </row>
     <row r="38" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -2787,11 +2778,11 @@
       <c r="H38" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I38" s="23" t="s">
+      <c r="I38" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
     </row>
     <row r="39" spans="1:11" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2821,8 +2812,8 @@
       <c r="I39" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -2852,8 +2843,8 @@
       <c r="I40" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -2880,11 +2871,11 @@
       <c r="H41" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I41" s="24" t="s">
+      <c r="I41" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
     </row>
     <row r="42" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
@@ -2908,14 +2899,14 @@
       <c r="G42" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
     </row>
     <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -2939,14 +2930,14 @@
       <c r="G43" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
     </row>
     <row r="44" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -2970,14 +2961,14 @@
       <c r="G44" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I44" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
@@ -3001,14 +2992,14 @@
       <c r="G45" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I45" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
     </row>
     <row r="46" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
@@ -3032,14 +3023,14 @@
       <c r="G46" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I46" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
     </row>
     <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
@@ -3063,14 +3054,14 @@
       <c r="G47" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I47" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
     </row>
     <row r="48" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -3094,14 +3085,14 @@
       <c r="G48" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I48" s="22" t="s">
+      <c r="H48" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I48" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
     </row>
     <row r="49" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -3125,14 +3116,14 @@
       <c r="G49" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H49" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I49" s="22" t="s">
+      <c r="H49" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
     </row>
     <row r="50" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
@@ -3156,14 +3147,14 @@
       <c r="G50" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H50" s="18" t="s">
+      <c r="H50" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
     </row>
     <row r="51" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
@@ -3187,14 +3178,14 @@
       <c r="G51" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
     </row>
     <row r="52" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
@@ -3218,14 +3209,14 @@
       <c r="G52" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H52" s="18" t="s">
+      <c r="H52" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
     </row>
     <row r="53" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -3249,14 +3240,14 @@
       <c r="G53" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H53" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
     </row>
     <row r="54" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -3280,14 +3271,14 @@
       <c r="G54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="18" t="s">
+      <c r="H54" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
     </row>
     <row r="55" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
@@ -3311,17 +3302,17 @@
       <c r="G55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I55" s="22" t="s">
+      <c r="H55" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
     </row>
     <row r="56" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="27" t="s">
         <v>139</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -3342,17 +3333,17 @@
       <c r="G56" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H56" s="18" t="s">
+      <c r="H56" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
     </row>
     <row r="57" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="28" t="s">
         <v>141</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3373,14 +3364,14 @@
       <c r="G57" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
     </row>
     <row r="58" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
@@ -3404,14 +3395,14 @@
       <c r="G58" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H58" s="18" t="s">
+      <c r="H58" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
     </row>
     <row r="59" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
@@ -3435,14 +3426,14 @@
       <c r="G59" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H59" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I59" s="22" t="s">
+      <c r="H59" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I59" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
     </row>
     <row r="60" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
@@ -3466,14 +3457,14 @@
       <c r="G60" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H60" s="18" t="s">
+      <c r="H60" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I60" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
     </row>
@@ -3499,14 +3490,14 @@
       <c r="G61" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H61" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I61" s="28" t="s">
+      <c r="H61" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I61" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="J61" s="22"/>
-      <c r="K61" s="22"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
     </row>
@@ -3515,7 +3506,7 @@
         <v>196</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>193</v>
@@ -3532,14 +3523,14 @@
       <c r="G62" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H62" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I62" s="29" t="s">
+      <c r="H62" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I62" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
     </row>
@@ -3548,7 +3539,7 @@
         <v>198</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>193</v>
@@ -3565,14 +3556,14 @@
       <c r="G63" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H63" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I63" s="29" t="s">
+      <c r="H63" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I63" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
     </row>
@@ -3581,7 +3572,7 @@
         <v>201</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>193</v>
@@ -3598,14 +3589,14 @@
       <c r="G64" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H64" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I64" s="28" t="s">
+      <c r="H64" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I64" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
     </row>
@@ -3631,7 +3622,7 @@
       <c r="G65" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H65" s="18" t="s">
+      <c r="H65" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I65" s="11" t="s">
@@ -3668,7 +3659,7 @@
       <c r="G66" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H66" s="18" t="s">
+      <c r="H66" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I66" s="11" t="s">
@@ -3705,14 +3696,14 @@
       <c r="G67" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H67" s="18" t="s">
+      <c r="H67" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
     </row>
@@ -3738,14 +3729,14 @@
       <c r="G68" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H68" s="18" t="s">
+      <c r="H68" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I68" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="J68" s="22"/>
-      <c r="K68" s="22"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
     </row>
@@ -3771,16 +3762,16 @@
       <c r="G69" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H69" s="18" t="s">
+      <c r="H69" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I69" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J69" s="22" t="s">
+      <c r="J69" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="K69" s="22" t="s">
+      <c r="K69" s="21" t="s">
         <v>163</v>
       </c>
       <c r="L69" s="5"/>
@@ -3808,7 +3799,7 @@
       <c r="G70" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H70" s="18" t="s">
+      <c r="H70" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I70" s="11" t="s">
@@ -3845,7 +3836,7 @@
       <c r="G71" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H71" s="18" t="s">
+      <c r="H71" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I71" s="11" t="s">
@@ -3882,7 +3873,7 @@
       <c r="G72" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H72" s="18" t="s">
+      <c r="H72" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I72" s="11" t="s">
@@ -3919,7 +3910,7 @@
       <c r="G73" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H73" s="18" t="s">
+      <c r="H73" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I73" s="11" t="s">
@@ -3956,14 +3947,14 @@
       <c r="G74" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H74" s="18" t="s">
+      <c r="H74" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I74" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="J74" s="25"/>
-      <c r="K74" s="25"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
       <c r="L74" s="13"/>
       <c r="M74" s="13"/>
     </row>
@@ -3989,171 +3980,171 @@
       <c r="G75" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H75" s="17" t="s">
         <v>53</v>
       </c>
       <c r="I75" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="J75" s="25"/>
-      <c r="K75" s="25"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
       <c r="L75" s="13"/>
       <c r="M75" s="13"/>
     </row>
     <row r="76" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="10" t="s">
         <v>176</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="17" t="s">
+      <c r="C76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E76" s="17">
-        <v>1</v>
-      </c>
-      <c r="F76" s="17">
-        <v>1</v>
-      </c>
-      <c r="G76" s="17" t="s">
+      <c r="E76" s="10">
+        <v>1</v>
+      </c>
+      <c r="F76" s="10">
+        <v>1</v>
+      </c>
+      <c r="G76" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H76" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I76" s="27" t="s">
+      <c r="H76" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I76" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="J76" s="20"/>
-      <c r="K76" s="20"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
     </row>
     <row r="77" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="10" t="s">
         <v>178</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C77" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D77" s="17" t="s">
+      <c r="C77" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D77" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E77" s="17">
-        <v>1</v>
-      </c>
-      <c r="F77" s="17">
-        <v>1</v>
-      </c>
-      <c r="G77" s="17" t="s">
+      <c r="E77" s="10">
+        <v>1</v>
+      </c>
+      <c r="F77" s="10">
+        <v>1</v>
+      </c>
+      <c r="G77" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H77" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I77" s="27" t="s">
+      <c r="H77" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I77" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="J77" s="20"/>
-      <c r="K77" s="20"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
     </row>
     <row r="78" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="10" t="s">
         <v>180</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D78" s="17" t="s">
+      <c r="C78" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D78" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E78" s="17">
-        <v>1</v>
-      </c>
-      <c r="F78" s="17">
-        <v>1</v>
-      </c>
-      <c r="G78" s="17" t="s">
+      <c r="E78" s="10">
+        <v>1</v>
+      </c>
+      <c r="F78" s="10">
+        <v>1</v>
+      </c>
+      <c r="G78" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H78" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I78" s="27" t="s">
+      <c r="H78" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I78" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="J78" s="20"/>
-      <c r="K78" s="20"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
     </row>
     <row r="79" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="10" t="s">
         <v>182</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C79" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="17">
-        <v>1</v>
-      </c>
-      <c r="F79" s="17">
-        <v>1</v>
-      </c>
-      <c r="G79" s="17" t="s">
+      <c r="C79" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="10">
+        <v>1</v>
+      </c>
+      <c r="F79" s="10">
+        <v>1</v>
+      </c>
+      <c r="G79" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H79" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I79" s="27" t="s">
+      <c r="H79" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I79" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="J79" s="20"/>
-      <c r="K79" s="20"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
     </row>
     <row r="80" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="10" t="s">
         <v>184</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C80" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="17">
-        <v>1</v>
-      </c>
-      <c r="F80" s="17">
+      <c r="C80" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="10">
+        <v>1</v>
+      </c>
+      <c r="F80" s="10">
         <v>4</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="G80" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H80" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I80" s="27" t="s">
+      <c r="H80" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I80" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="J80" s="20"/>
-      <c r="K80" s="20"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified Classes and ,methods for regression
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\101222_Web\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\101922_Web\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE188E54-DD10-4D91-93ED-18AC74EFD9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5135A4-DE4B-4A96-9D42-03E3C5568F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -902,15 +902,6 @@
     <t>verify Buy Token Trasactions Credit Card WithOut Payment</t>
   </si>
   <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testBuyTokenTransactionsWithoutBankAccount,
--pexpBankName,
--pexpUserName,
--pexpPassword,
--pamount,
--pcode</t>
-  </si>
-  <si>
     <t>test Forgot Password</t>
   </si>
   <si>
@@ -1450,13 +1441,6 @@
   </si>
   <si>
     <t>Verify WithdrawToUSD  Add Bank Account</t>
-  </si>
-  <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testWithdrawToUSDAddExternalBankAccount,
--pexpBankName,
--pexpUserName,
--pexpPassword</t>
   </si>
   <si>
     <t>coyni.customer.tests.TokenAccountTest,
@@ -1713,6 +1697,24 @@
   <si>
     <t>coyni.customer.tests.PaymentMethodsTest,
 testAddBankAccountWithOutPaymentMethod,
+-proutingNumber,
+-pconfirmRouting,
+-paccountNumber,
+-pconfirmAccountNumber</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testBuyTokenTransactionsWithoutBankAccount,
+-proutingNumber,
+-pconfirmRouting,
+-paccountNumber,
+-pconfirmAccountNumber,
+-pamount,
+-pcode</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testWithdrawToUSDAddExternalBankAccount,
 -proutingNumber,
 -pconfirmRouting,
 -paccountNumber,
@@ -2199,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,7 +2299,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -2355,7 +2357,7 @@
     </row>
     <row r="6" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>44</v>
@@ -2376,7 +2378,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -2384,7 +2386,7 @@
     </row>
     <row r="7" spans="1:11" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>44</v>
@@ -2405,7 +2407,7 @@
         <v>23</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -2413,7 +2415,7 @@
     </row>
     <row r="8" spans="1:11" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>44</v>
@@ -2434,7 +2436,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -2463,7 +2465,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="28"/>
@@ -2637,13 +2639,13 @@
     </row>
     <row r="16" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>191</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>76</v>
@@ -2655,21 +2657,21 @@
         <v>13</v>
       </c>
       <c r="G16" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>12</v>
@@ -2681,21 +2683,21 @@
         <v>31</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>76</v>
@@ -2707,21 +2709,21 @@
         <v>13</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>12</v>
@@ -2733,10 +2735,10 @@
         <v>27</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -2939,7 +2941,7 @@
         <v>184</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -2968,7 +2970,7 @@
         <v>184</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -3055,7 +3057,7 @@
         <v>184</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -3084,12 +3086,12 @@
         <v>184</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>44</v>
@@ -3113,7 +3115,7 @@
         <v>184</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -3142,7 +3144,7 @@
         <v>184</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3200,7 +3202,7 @@
         <v>184</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3229,7 +3231,7 @@
         <v>184</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3292,7 +3294,7 @@
     </row>
     <row r="39" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>44</v>
@@ -3316,12 +3318,12 @@
         <v>184</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>44</v>
@@ -3345,7 +3347,7 @@
         <v>184</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3434,7 +3436,7 @@
         <v>184</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J43" s="7"/>
     </row>
@@ -3443,7 +3445,7 @@
         <v>82</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>180</v>
@@ -3464,7 +3466,7 @@
         <v>184</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J44" s="7"/>
     </row>
@@ -3494,7 +3496,7 @@
         <v>184</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J45" s="7"/>
     </row>
@@ -3524,7 +3526,7 @@
         <v>184</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46" s="7"/>
     </row>
@@ -3554,7 +3556,7 @@
         <v>184</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J47" s="7"/>
     </row>
@@ -3614,7 +3616,7 @@
         <v>184</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J49" s="7"/>
     </row>
@@ -3734,7 +3736,7 @@
         <v>184</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J53" s="7"/>
     </row>
@@ -3859,10 +3861,10 @@
         <v>110</v>
       </c>
       <c r="K57" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="L57" s="21" t="s">
         <v>215</v>
-      </c>
-      <c r="L57" s="21" t="s">
-        <v>216</v>
       </c>
       <c r="M57" s="22"/>
       <c r="N57" s="22"/>
@@ -3899,10 +3901,10 @@
         <v>110</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L58" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
@@ -4007,7 +4009,7 @@
         <v>110</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>117</v>
@@ -4047,10 +4049,10 @@
         <v>110</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L62" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M62" s="22"/>
       <c r="N62" s="22"/>
@@ -4087,7 +4089,7 @@
         <v>110</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L63" s="21" t="s">
         <v>120</v>
@@ -4121,13 +4123,13 @@
         <v>184</v>
       </c>
       <c r="I64" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J64" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L64" s="21" t="s">
         <v>122</v>
@@ -4167,10 +4169,10 @@
         <v>110</v>
       </c>
       <c r="K65" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L65" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M65" s="22"/>
       <c r="N65" s="22"/>
@@ -4355,7 +4357,7 @@
         <v>184</v>
       </c>
       <c r="I71" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J71" s="7"/>
     </row>
@@ -4385,7 +4387,7 @@
         <v>184</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
@@ -4418,7 +4420,7 @@
         <v>184</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -4451,7 +4453,7 @@
         <v>184</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>189</v>
+        <v>283</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -4484,7 +4486,7 @@
         <v>184</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
@@ -4517,7 +4519,7 @@
         <v>184</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
@@ -4550,7 +4552,7 @@
         <v>184</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -4583,7 +4585,7 @@
         <v>184</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
@@ -4649,7 +4651,7 @@
         <v>184</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
@@ -4682,7 +4684,7 @@
         <v>184</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -4694,7 +4696,7 @@
         <v>154</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>182</v>
@@ -4715,7 +4717,7 @@
         <v>184</v>
       </c>
       <c r="I82" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="219" customHeight="1" x14ac:dyDescent="0.25">
@@ -4723,7 +4725,7 @@
         <v>157</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>182</v>
@@ -4744,15 +4746,15 @@
         <v>184</v>
       </c>
       <c r="I83" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>182</v>
@@ -4773,7 +4775,7 @@
         <v>184</v>
       </c>
       <c r="I84" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4781,7 +4783,7 @@
         <v>158</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>182</v>
@@ -4810,7 +4812,7 @@
         <v>152</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>182</v>
@@ -4843,7 +4845,7 @@
         <v>150</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>182</v>
@@ -4876,7 +4878,7 @@
         <v>148</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>182</v>
@@ -4897,7 +4899,7 @@
         <v>184</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
@@ -4909,7 +4911,7 @@
         <v>155</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>182</v>
@@ -4930,7 +4932,7 @@
         <v>184</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="135" x14ac:dyDescent="0.25">
@@ -4938,7 +4940,7 @@
         <v>156</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>182</v>
@@ -4959,7 +4961,7 @@
         <v>184</v>
       </c>
       <c r="I90" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="135" x14ac:dyDescent="0.25">
@@ -4967,7 +4969,7 @@
         <v>160</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>180</v>
@@ -4993,10 +4995,10 @@
     </row>
     <row r="92" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>180</v>
@@ -5017,7 +5019,7 @@
         <v>184</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="180" x14ac:dyDescent="0.25">
@@ -5025,7 +5027,7 @@
         <v>162</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>163</v>
@@ -5046,7 +5048,7 @@
         <v>184</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
@@ -5058,7 +5060,7 @@
         <v>165</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>163</v>
@@ -5091,7 +5093,7 @@
         <v>167</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>163</v>
@@ -5112,7 +5114,7 @@
         <v>184</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
@@ -5124,7 +5126,7 @@
         <v>168</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>163</v>
@@ -5157,7 +5159,7 @@
         <v>170</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>180</v>
@@ -5241,13 +5243,13 @@
     </row>
     <row r="100" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>76</v>
@@ -5259,7 +5261,7 @@
         <v>13</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>184</v>
@@ -5270,13 +5272,13 @@
     </row>
     <row r="101" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>76</v>
@@ -5288,24 +5290,24 @@
         <v>13</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I101" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>76</v>
@@ -5317,24 +5319,24 @@
         <v>13</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I102" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>12</v>
@@ -5346,24 +5348,24 @@
         <v>33</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H103" s="15" t="s">
         <v>184</v>
       </c>
       <c r="I103" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>12</v>
@@ -5375,53 +5377,53 @@
         <v>13</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H104" s="15" t="s">
         <v>184</v>
       </c>
       <c r="I104" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="11" t="s">
-        <v>234</v>
-      </c>
       <c r="G105" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H105" s="15" t="s">
         <v>184</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>12</v>
@@ -5433,53 +5435,53 @@
         <v>27</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H106" s="15" t="s">
         <v>184</v>
       </c>
       <c r="I106" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H107" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="I107" s="13" t="s">
         <v>264</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C107" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="I107" s="13" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C108" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>12</v>
@@ -5491,24 +5493,24 @@
         <v>13</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H108" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C109" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>12</v>
@@ -5520,24 +5522,24 @@
         <v>13</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>12</v>
@@ -5549,24 +5551,24 @@
         <v>139</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H110" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I110" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>12</v>
@@ -5578,13 +5580,13 @@
         <v>13</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I111" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified methods for percentage calculation of trasaction
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\101922_Web\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5135A4-DE4B-4A96-9D42-03E3C5568F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D47AC-D5B6-4B46-A912-A6D113238427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -657,19 +657,6 @@
     <t>test gift card navigation</t>
   </si>
   <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testWithdrawToUSDNavigationOption,
--pgiftHeading,
--pfirstName,
--plastName,
--pemail,
--pamount,
--porderHeading,
--pauthyHeading1,
--psecurityKey,
--psuccessHeading</t>
-  </si>
-  <si>
     <t>test gift card amazon  with invalid data</t>
   </si>
   <si>
@@ -1114,21 +1101,6 @@
 -perrMessage</t>
   </si>
   <si>
-    <t>coyni.customer.tests.TokenAccountTest,
-testWithdrawToUSDViaInstantPayWithPayment,
--pcssProp,
--pexpValue,
--pexpColor,
--pwithdrawToUSDHeading,
--pinstantPayHeading,
--plast4digits,
--pamount,
--ptransactionalmessage,
--pauthyVerificationHeading,
--psecurityKey,
--pexpTransactionInProgressHeading</t>
-  </si>
-  <si>
     <t>coyni.customer.tests.CustomerProfileTest,
 testPreferencesSelectTimeZone,
 -pexpColor,
@@ -1719,6 +1691,35 @@
 -pconfirmRouting,
 -paccountNumber,
 -pconfirmAccountNumber</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testWithdrawToUSDNavigationOption,
+-pgiftHeading,
+-pfirstName,
+-plastName,
+-pemail,
+-pemail1,
+-pamount,
+-porderHeading,
+-pauthyHeading1,
+-psecurityKey,
+-psuccessHeading</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testWithdrawToUSDViaInstantPay,
+-pcssProp,
+-pexpValue,
+-pexpColor,
+-pwithdrawToUSDHeading,
+-pinstantPayHeading,
+-plast4digits,
+-pamount,
+-ptransactionalmessage,
+-pauthyVerificationHeading,
+-pcode,
+-pexpTransactionInProgressHeading</t>
   </si>
 </sst>
 </file>
@@ -2201,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +2273,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I2" s="4"/>
     </row>
@@ -2299,7 +2300,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -2357,7 +2358,7 @@
     </row>
     <row r="6" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>44</v>
@@ -2378,7 +2379,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -2386,7 +2387,7 @@
     </row>
     <row r="7" spans="1:11" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>44</v>
@@ -2407,7 +2408,7 @@
         <v>23</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -2415,7 +2416,7 @@
     </row>
     <row r="8" spans="1:11" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>44</v>
@@ -2436,7 +2437,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -2465,7 +2466,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="28"/>
@@ -2633,19 +2634,19 @@
         <v>30</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>189</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>190</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>76</v>
@@ -2657,21 +2658,21 @@
         <v>13</v>
       </c>
       <c r="G16" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>12</v>
@@ -2683,21 +2684,21 @@
         <v>31</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>76</v>
@@ -2709,21 +2710,21 @@
         <v>13</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>12</v>
@@ -2735,10 +2736,10 @@
         <v>27</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -2749,7 +2750,7 @@
         <v>44</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
@@ -2764,7 +2765,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>42</v>
@@ -2778,7 +2779,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>12</v>
@@ -2793,7 +2794,7 @@
         <v>41</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>45</v>
@@ -2807,7 +2808,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>12</v>
@@ -2822,7 +2823,7 @@
         <v>41</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>47</v>
@@ -2836,7 +2837,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>12</v>
@@ -2851,7 +2852,7 @@
         <v>41</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>49</v>
@@ -2865,7 +2866,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>12</v>
@@ -2880,7 +2881,7 @@
         <v>51</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>52</v>
@@ -2894,7 +2895,7 @@
         <v>44</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>12</v>
@@ -2909,7 +2910,7 @@
         <v>51</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>54</v>
@@ -2938,10 +2939,10 @@
         <v>57</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -2967,10 +2968,10 @@
         <v>57</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -2996,7 +2997,7 @@
         <v>57</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>58</v>
@@ -3025,7 +3026,7 @@
         <v>57</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>70</v>
@@ -3054,10 +3055,10 @@
         <v>57</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -3083,15 +3084,15 @@
         <v>57</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>44</v>
@@ -3112,10 +3113,10 @@
         <v>57</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -3141,10 +3142,10 @@
         <v>57</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3170,7 +3171,7 @@
         <v>57</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>65</v>
@@ -3199,10 +3200,10 @@
         <v>57</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3228,10 +3229,10 @@
         <v>57</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3257,7 +3258,7 @@
         <v>57</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I37" s="15" t="s">
         <v>72</v>
@@ -3286,7 +3287,7 @@
         <v>57</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>74</v>
@@ -3294,7 +3295,7 @@
     </row>
     <row r="39" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>44</v>
@@ -3315,15 +3316,15 @@
         <v>57</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>44</v>
@@ -3344,10 +3345,10 @@
         <v>57</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3358,7 +3359,7 @@
         <v>44</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>76</v>
@@ -3373,7 +3374,7 @@
         <v>77</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>78</v>
@@ -3388,7 +3389,7 @@
         <v>44</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>76</v>
@@ -3403,7 +3404,7 @@
         <v>77</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>80</v>
@@ -3418,7 +3419,7 @@
         <v>44</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>76</v>
@@ -3433,10 +3434,10 @@
         <v>77</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J43" s="7"/>
     </row>
@@ -3448,7 +3449,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>76</v>
@@ -3463,10 +3464,10 @@
         <v>83</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J44" s="7"/>
     </row>
@@ -3478,7 +3479,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>76</v>
@@ -3493,10 +3494,10 @@
         <v>85</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J45" s="7"/>
     </row>
@@ -3508,7 +3509,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>76</v>
@@ -3523,10 +3524,10 @@
         <v>87</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J46" s="7"/>
     </row>
@@ -3538,7 +3539,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>76</v>
@@ -3553,10 +3554,10 @@
         <v>89</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J47" s="7"/>
     </row>
@@ -3568,7 +3569,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>76</v>
@@ -3583,7 +3584,7 @@
         <v>91</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>92</v>
@@ -3598,7 +3599,7 @@
         <v>44</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>76</v>
@@ -3613,10 +3614,10 @@
         <v>41</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J49" s="7"/>
     </row>
@@ -3628,7 +3629,7 @@
         <v>44</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>76</v>
@@ -3643,7 +3644,7 @@
         <v>41</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I50" s="21" t="s">
         <v>95</v>
@@ -3658,7 +3659,7 @@
         <v>44</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>12</v>
@@ -3673,7 +3674,7 @@
         <v>41</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I51" s="21" t="s">
         <v>97</v>
@@ -3688,7 +3689,7 @@
         <v>44</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>76</v>
@@ -3703,7 +3704,7 @@
         <v>41</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I52" s="21" t="s">
         <v>99</v>
@@ -3718,7 +3719,7 @@
         <v>44</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>12</v>
@@ -3733,10 +3734,10 @@
         <v>41</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J53" s="7"/>
     </row>
@@ -3748,7 +3749,7 @@
         <v>44</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>76</v>
@@ -3763,7 +3764,7 @@
         <v>41</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I54" s="21" t="s">
         <v>102</v>
@@ -3778,7 +3779,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>76</v>
@@ -3793,7 +3794,7 @@
         <v>41</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I55" s="21" t="s">
         <v>104</v>
@@ -3808,7 +3809,7 @@
         <v>44</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>76</v>
@@ -3823,7 +3824,7 @@
         <v>106</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I56" s="21" t="s">
         <v>107</v>
@@ -3837,7 +3838,7 @@
         <v>44</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>12</v>
@@ -3852,19 +3853,19 @@
         <v>109</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J57" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K57" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="L57" s="21" t="s">
         <v>214</v>
-      </c>
-      <c r="L57" s="21" t="s">
-        <v>215</v>
       </c>
       <c r="M57" s="22"/>
       <c r="N57" s="22"/>
@@ -3877,7 +3878,7 @@
         <v>44</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D58" s="31" t="s">
         <v>12</v>
@@ -3892,19 +3893,19 @@
         <v>109</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J58" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L58" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
@@ -3917,7 +3918,7 @@
         <v>44</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>12</v>
@@ -3932,7 +3933,7 @@
         <v>109</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I59" s="21" t="s">
         <v>113</v>
@@ -3951,7 +3952,7 @@
         <v>44</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>12</v>
@@ -3966,7 +3967,7 @@
         <v>109</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I60" s="21" t="s">
         <v>115</v>
@@ -3985,7 +3986,7 @@
         <v>44</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>12</v>
@@ -4000,16 +4001,16 @@
         <v>109</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I61" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J61" s="8" t="s">
         <v>110</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>117</v>
@@ -4025,7 +4026,7 @@
         <v>44</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>12</v>
@@ -4040,19 +4041,19 @@
         <v>109</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I62" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J62" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L62" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M62" s="22"/>
       <c r="N62" s="22"/>
@@ -4065,7 +4066,7 @@
         <v>44</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>12</v>
@@ -4080,16 +4081,16 @@
         <v>109</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I63" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J63" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L63" s="21" t="s">
         <v>120</v>
@@ -4105,7 +4106,7 @@
         <v>44</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>12</v>
@@ -4120,16 +4121,16 @@
         <v>109</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I64" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J64" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L64" s="21" t="s">
         <v>122</v>
@@ -4145,7 +4146,7 @@
         <v>44</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>12</v>
@@ -4160,19 +4161,19 @@
         <v>109</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I65" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J65" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K65" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L65" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M65" s="22"/>
       <c r="N65" s="22"/>
@@ -4185,7 +4186,7 @@
         <v>44</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D66" s="22" t="s">
         <v>12</v>
@@ -4200,7 +4201,7 @@
         <v>109</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>125</v>
@@ -4219,7 +4220,7 @@
         <v>44</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>76</v>
@@ -4234,7 +4235,7 @@
         <v>109</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>127</v>
@@ -4249,7 +4250,7 @@
         <v>44</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>76</v>
@@ -4264,7 +4265,7 @@
         <v>109</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I68" s="8" t="s">
         <v>129</v>
@@ -4279,7 +4280,7 @@
         <v>44</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>76</v>
@@ -4294,7 +4295,7 @@
         <v>109</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I69" s="8" t="s">
         <v>131</v>
@@ -4309,7 +4310,7 @@
         <v>44</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>12</v>
@@ -4324,7 +4325,7 @@
         <v>109</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I70" s="8" t="s">
         <v>133</v>
@@ -4339,7 +4340,7 @@
         <v>44</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>12</v>
@@ -4354,10 +4355,10 @@
         <v>109</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I71" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J71" s="7"/>
     </row>
@@ -4384,10 +4385,10 @@
         <v>137</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
@@ -4417,10 +4418,10 @@
         <v>137</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -4429,13 +4430,13 @@
     </row>
     <row r="74" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D74" s="22" t="s">
         <v>12</v>
@@ -4450,10 +4451,10 @@
         <v>41</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -4462,13 +4463,13 @@
     </row>
     <row r="75" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D75" s="22" t="s">
         <v>12</v>
@@ -4483,10 +4484,10 @@
         <v>41</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
@@ -4495,13 +4496,13 @@
     </row>
     <row r="76" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>12</v>
@@ -4516,10 +4517,10 @@
         <v>41</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
@@ -4549,10 +4550,10 @@
         <v>142</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -4582,17 +4583,17 @@
         <v>142</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>144</v>
       </c>
@@ -4615,10 +4616,10 @@
         <v>142</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>145</v>
+        <v>283</v>
       </c>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -4627,7 +4628,7 @@
     </row>
     <row r="80" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>44</v>
@@ -4648,10 +4649,10 @@
         <v>142</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
@@ -4660,7 +4661,7 @@
     </row>
     <row r="81" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>44</v>
@@ -4681,10 +4682,10 @@
         <v>142</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -4693,13 +4694,13 @@
     </row>
     <row r="82" spans="1:13" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D82" s="22" t="s">
         <v>12</v>
@@ -4711,24 +4712,24 @@
         <v>1</v>
       </c>
       <c r="G82" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I82" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="219" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D83" s="22" t="s">
         <v>12</v>
@@ -4740,24 +4741,24 @@
         <v>1</v>
       </c>
       <c r="G83" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I83" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>12</v>
@@ -4769,24 +4770,24 @@
         <v>17</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I84" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D85" s="22" t="s">
         <v>12</v>
@@ -4798,42 +4799,42 @@
         <v>4</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I85" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" s="7">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7">
+        <v>1</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I86" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="7">
-        <v>1</v>
-      </c>
-      <c r="F86" s="7">
-        <v>1</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I86" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
@@ -4842,13 +4843,13 @@
     </row>
     <row r="87" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>12</v>
@@ -4860,28 +4861,28 @@
         <v>31</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>12</v>
@@ -4893,13 +4894,13 @@
         <v>1</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>219</v>
+        <v>284</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
@@ -4908,13 +4909,13 @@
     </row>
     <row r="89" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D89" s="22" t="s">
         <v>12</v>
@@ -4926,24 +4927,24 @@
         <v>1</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>12</v>
@@ -4955,24 +4956,24 @@
         <v>1</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I90" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>12</v>
@@ -4987,21 +4988,21 @@
         <v>41</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>12</v>
@@ -5016,21 +5017,21 @@
         <v>41</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>76</v>
@@ -5042,13 +5043,13 @@
         <v>1</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
@@ -5057,31 +5058,31 @@
     </row>
     <row r="94" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="7">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I94" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" s="7">
-        <v>1</v>
-      </c>
-      <c r="F94" s="7">
-        <v>1</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I94" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
@@ -5090,13 +5091,13 @@
     </row>
     <row r="95" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>76</v>
@@ -5108,13 +5109,13 @@
         <v>1</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
@@ -5123,13 +5124,13 @@
     </row>
     <row r="96" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>76</v>
@@ -5141,13 +5142,13 @@
         <v>1</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
@@ -5156,13 +5157,13 @@
     </row>
     <row r="97" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>12</v>
@@ -5177,79 +5178,79 @@
         <v>41</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C98" s="25" t="s">
+      <c r="D98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F98" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G98" s="2" t="s">
+      <c r="H98" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I98" s="24" t="s">
         <v>175</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I98" s="24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I99" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C99" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E99" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H99" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I99" s="24" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>76</v>
@@ -5261,24 +5262,24 @@
         <v>13</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I100" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>76</v>
@@ -5290,24 +5291,24 @@
         <v>13</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I101" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>76</v>
@@ -5319,24 +5320,24 @@
         <v>13</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I102" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>12</v>
@@ -5348,24 +5349,24 @@
         <v>33</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I103" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>12</v>
@@ -5377,24 +5378,24 @@
         <v>13</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I104" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>12</v>
@@ -5403,27 +5404,27 @@
         <v>13</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H105" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>12</v>
@@ -5435,53 +5436,53 @@
         <v>27</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H106" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I106" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H107" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="I107" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C107" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="I107" s="13" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C108" s="33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>12</v>
@@ -5493,24 +5494,24 @@
         <v>13</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H108" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C109" s="33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>12</v>
@@ -5522,24 +5523,24 @@
         <v>13</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>12</v>
@@ -5551,24 +5552,24 @@
         <v>139</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I110" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>12</v>
@@ -5577,16 +5578,16 @@
         <v>13</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I111" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5645,7 +5646,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data and Test Script for Customer Portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript.xlsx
+++ b/Web/coyni/resources/TestScript.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\101922_Web\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_web_2.3\clone_Merchant_2.3_20_02_2023\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D47AC-D5B6-4B46-A912-A6D113238427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434505F6-A525-4493-B08D-C6C34389FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$113</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="291">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1720,6 +1720,52 @@
 -pauthyVerificationHeading,
 -pcode,
 -pexpTransactionInProgressHeading</t>
+  </si>
+  <si>
+    <t>customer Get Started</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.SignupTest,
+testSignUpBusinessViaIndividual,
+-pheading</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testUserDetailsAddress,
+-paddress1,
+-paddress2,
+-pcity,
+-pstate,
+-pzipcode,
+-pcreatePassword,
+-pemail</t>
+  </si>
+  <si>
+    <t>verify add card</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLogin,
+-ploginHeading,
+-pemail,
+-ppassword,
+-pauthyHeading,
+-pcode</t>
+  </si>
+  <si>
+    <t>coyni.customer.tests.TokenAccountTest,
+testAddDebitCard,
+-pnameOnCard,
+-pcardNumber,
+-pcardType,
+-pcardExpiry,
+-pcvvNumber,
+-paddress1,
+-paddress2,
+-pcity,
+-pzipCode,
+-pstate,
+-pamount</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1885,6 +1931,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2200,28 +2249,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}">
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
-    <col min="8" max="8" width="51.42578125" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="41.85546875" customWidth="1"/>
-    <col min="12" max="12" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" customWidth="1"/>
+    <col min="9" max="9" width="44.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="41.88671875" customWidth="1"/>
+    <col min="12" max="12" width="41.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2277,9 +2326,9 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="137.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>285</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>44</v>
@@ -2288,7 +2337,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>13</v>
@@ -2300,13 +2349,15 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="163.35" customHeight="1" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>288</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>44</v>
@@ -2315,24 +2366,27 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>44</v>
@@ -2353,70 +2407,67 @@
         <v>14</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="163.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="103.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="8" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>44</v>
@@ -2425,27 +2476,27 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="136.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>44</v>
@@ -2460,21 +2511,21 @@
         <v>13</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="I9" s="27"/>
+        <v>200</v>
+      </c>
+      <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>201</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>44</v>
@@ -2489,21 +2540,21 @@
         <v>13</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="27"/>
+        <v>202</v>
+      </c>
+      <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>44</v>
@@ -2518,75 +2569,79 @@
         <v>13</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>44</v>
@@ -2607,13 +2662,13 @@
         <v>30</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>44</v>
@@ -2634,65 +2689,67 @@
         <v>30</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>188</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>192</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>194</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>44</v>
@@ -2713,12 +2770,12 @@
         <v>190</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>44</v>
@@ -2726,83 +2783,77 @@
       <c r="C19" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="26" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G19" s="26" t="s">
         <v>190</v>
       </c>
       <c r="H19" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>44</v>
@@ -2826,12 +2877,12 @@
         <v>183</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>44</v>
@@ -2855,12 +2906,12 @@
         <v>183</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>44</v>
@@ -2878,18 +2929,18 @@
         <v>13</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>183</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>44</v>
@@ -2907,76 +2958,76 @@
         <v>13</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I25" s="8" t="s">
+      <c r="H26" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="28" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="I26" s="13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>44</v>
@@ -2990,8 +3041,8 @@
       <c r="E28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="2">
-        <v>1</v>
+      <c r="F28" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>57</v>
@@ -3000,41 +3051,41 @@
         <v>183</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>69</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="17" t="s">
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>59</v>
+      <c r="H29" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>44</v>
@@ -3048,8 +3099,8 @@
       <c r="E30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>13</v>
+      <c r="F30" s="2">
+        <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>57</v>
@@ -3058,47 +3109,47 @@
         <v>183</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="D31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="17" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>259</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>12</v>
@@ -3106,8 +3157,8 @@
       <c r="E32" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>17</v>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>57</v>
@@ -3116,70 +3167,70 @@
         <v>183</v>
       </c>
       <c r="I32" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="I34" s="13" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="240" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="35" spans="1:10" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>44</v>
@@ -3199,103 +3250,103 @@
       <c r="G35" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I35" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
         <v>64</v>
       </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="I36" s="5" t="s">
+      <c r="H38" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I38" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="39" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>236</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>44</v>
@@ -3318,13 +3369,13 @@
       <c r="H39" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="I39" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>237</v>
+        <v>73</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>44</v>
@@ -3348,72 +3399,70 @@
         <v>183</v>
       </c>
       <c r="I40" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I42" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="43" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I41" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" s="7">
-        <v>1</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="J42" s="7"/>
-    </row>
-    <row r="43" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>44</v>
@@ -3437,13 +3486,13 @@
         <v>183</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>218</v>
+        <v>78</v>
       </c>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>82</v>
+    <row r="44" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>44</v>
@@ -3461,19 +3510,19 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>219</v>
+        <v>80</v>
       </c>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>84</v>
+    <row r="45" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>44</v>
@@ -3491,19 +3540,19 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>44</v>
@@ -3521,19 +3570,19 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>44</v>
@@ -3551,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>183</v>
@@ -3561,9 +3610,9 @@
       </c>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>44</v>
@@ -3581,19 +3630,19 @@
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I48" s="8" t="s">
-        <v>92</v>
+      <c r="I48" s="21" t="s">
+        <v>220</v>
       </c>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>44</v>
@@ -3611,19 +3660,19 @@
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I49" s="8" t="s">
-        <v>212</v>
+      <c r="I49" s="21" t="s">
+        <v>220</v>
       </c>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>44</v>
@@ -3641,19 +3690,19 @@
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I50" s="21" t="s">
-        <v>95</v>
+      <c r="I50" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>44</v>
@@ -3662,13 +3711,13 @@
         <v>179</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E51" s="7">
         <v>1</v>
       </c>
       <c r="F51" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>41</v>
@@ -3676,14 +3725,14 @@
       <c r="H51" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I51" s="21" t="s">
-        <v>97</v>
+      <c r="I51" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>44</v>
@@ -3707,13 +3756,13 @@
         <v>183</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J52" s="7"/>
     </row>
-    <row r="53" spans="1:14" ht="150" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>100</v>
+    <row r="53" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>44</v>
@@ -3728,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>41</v>
@@ -3736,14 +3785,14 @@
       <c r="H53" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>272</v>
+      <c r="I53" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>44</v>
@@ -3767,13 +3816,13 @@
         <v>183</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
-        <v>103</v>
+    <row r="55" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>44</v>
@@ -3782,7 +3831,7 @@
         <v>179</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="E55" s="7">
         <v>1</v>
@@ -3796,14 +3845,14 @@
       <c r="H55" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I55" s="21" t="s">
-        <v>104</v>
+      <c r="I55" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>44</v>
@@ -3821,166 +3870,158 @@
         <v>1</v>
       </c>
       <c r="G56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I56" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7">
+        <v>1</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I57" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7">
+        <v>1</v>
+      </c>
+      <c r="G58" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I56" s="21" t="s">
+      <c r="H58" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I58" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="4" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
+    <row r="59" spans="1:14" s="4" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="32" t="s">
+      <c r="B59" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="22">
-        <v>1</v>
-      </c>
-      <c r="F57" s="22">
-        <v>1</v>
-      </c>
-      <c r="G57" s="22" t="s">
+      <c r="D59" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="22">
+        <v>1</v>
+      </c>
+      <c r="F59" s="22">
+        <v>1</v>
+      </c>
+      <c r="G59" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="H57" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I57" s="21" t="s">
+      <c r="H59" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I59" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J57" s="21" t="s">
+      <c r="J59" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="K57" s="21" t="s">
+      <c r="K59" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="L57" s="21" t="s">
+      <c r="L59" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="M57" s="22"/>
-      <c r="N57" s="22"/>
-    </row>
-    <row r="58" spans="1:14" s="4" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31" t="s">
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+    </row>
+    <row r="60" spans="1:14" s="4" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="32" t="s">
+      <c r="B60" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="D58" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="22">
-        <v>1</v>
-      </c>
-      <c r="F58" s="22">
-        <v>1</v>
-      </c>
-      <c r="G58" s="22" t="s">
+      <c r="D60" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="22">
+        <v>1</v>
+      </c>
+      <c r="F60" s="22">
+        <v>1</v>
+      </c>
+      <c r="G60" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="H58" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I58" s="21" t="s">
+      <c r="H60" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I60" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J58" s="21" t="s">
+      <c r="J60" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="K58" s="21" t="s">
+      <c r="K60" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="L58" s="21" t="s">
+      <c r="L60" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="M58" s="21"/>
-      <c r="N58" s="21"/>
-    </row>
-    <row r="59" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+    </row>
+    <row r="61" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="7">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7">
-        <v>1</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I59" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="8"/>
-    </row>
-    <row r="60" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="7">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7">
-        <v>1</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I60" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
-    </row>
-    <row r="61" spans="1:14" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>44</v>
@@ -4004,23 +4045,17 @@
         <v>183</v>
       </c>
       <c r="I61" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="J61" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="K61" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="L61" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="M61" s="7"/>
-      <c r="N61" s="7"/>
-    </row>
-    <row r="62" spans="1:14" s="4" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+    </row>
+    <row r="62" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>44</v>
@@ -4028,39 +4063,33 @@
       <c r="C62" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D62" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="22">
-        <v>1</v>
-      </c>
-      <c r="F62" s="22">
-        <v>1</v>
-      </c>
-      <c r="G62" s="22" t="s">
+      <c r="D62" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="7">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7">
+        <v>1</v>
+      </c>
+      <c r="G62" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I62" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="J62" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="K62" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="L62" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-    </row>
-    <row r="63" spans="1:14" s="4" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+    </row>
+    <row r="63" spans="1:14" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>44</v>
@@ -4068,16 +4097,16 @@
       <c r="C63" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D63" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="22">
-        <v>1</v>
-      </c>
-      <c r="F63" s="22">
-        <v>1</v>
-      </c>
-      <c r="G63" s="22" t="s">
+      <c r="D63" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="7">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7">
+        <v>1</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H63" s="5" t="s">
@@ -4086,21 +4115,21 @@
       <c r="I63" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J63" s="21" t="s">
+      <c r="J63" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="K63" s="21" t="s">
+      <c r="K63" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L63" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-    </row>
-    <row r="64" spans="1:14" s="4" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="21" t="s">
-        <v>121</v>
+      <c r="L63" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+    </row>
+    <row r="64" spans="1:14" s="4" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>44</v>
@@ -4124,7 +4153,7 @@
         <v>183</v>
       </c>
       <c r="I64" s="21" t="s">
-        <v>256</v>
+        <v>182</v>
       </c>
       <c r="J64" s="21" t="s">
         <v>110</v>
@@ -4133,14 +4162,14 @@
         <v>246</v>
       </c>
       <c r="L64" s="21" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="M64" s="22"/>
       <c r="N64" s="22"/>
     </row>
-    <row r="65" spans="1:14" s="4" customFormat="1" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="4" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>44</v>
@@ -4173,14 +4202,14 @@
         <v>246</v>
       </c>
       <c r="L65" s="21" t="s">
-        <v>257</v>
+        <v>120</v>
       </c>
       <c r="M65" s="22"/>
       <c r="N65" s="22"/>
     </row>
-    <row r="66" spans="1:14" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="s">
-        <v>124</v>
+    <row r="66" spans="1:14" s="4" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>44</v>
@@ -4204,77 +4233,97 @@
         <v>183</v>
       </c>
       <c r="I66" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="J66" s="22"/>
-      <c r="K66" s="22"/>
-      <c r="L66" s="22"/>
+        <v>256</v>
+      </c>
+      <c r="J66" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="K66" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="L66" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="M66" s="22"/>
       <c r="N66" s="22"/>
     </row>
-    <row r="67" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="67" spans="1:14" s="4" customFormat="1" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="22">
+        <v>1</v>
+      </c>
+      <c r="F67" s="22">
+        <v>1</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I67" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="J67" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="K67" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="L67" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="M67" s="22"/>
+      <c r="N67" s="22"/>
+    </row>
+    <row r="68" spans="1:14" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="22">
+        <v>1</v>
+      </c>
+      <c r="F68" s="22">
+        <v>1</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+      <c r="L68" s="22"/>
+      <c r="M68" s="22"/>
+      <c r="N68" s="22"/>
+    </row>
+    <row r="69" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="7">
-        <v>1</v>
-      </c>
-      <c r="F67" s="7">
-        <v>1</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J67" s="7"/>
-    </row>
-    <row r="68" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E68" s="7">
-        <v>1</v>
-      </c>
-      <c r="F68" s="7">
-        <v>1</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="J68" s="7"/>
-    </row>
-    <row r="69" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>44</v>
@@ -4298,13 +4347,13 @@
         <v>183</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>44</v>
@@ -4313,12 +4362,12 @@
         <v>180</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="9">
-        <v>1</v>
-      </c>
-      <c r="F70" s="9">
+        <v>76</v>
+      </c>
+      <c r="E70" s="7">
+        <v>1</v>
+      </c>
+      <c r="F70" s="7">
         <v>1</v>
       </c>
       <c r="G70" s="7" t="s">
@@ -4328,13 +4377,13 @@
         <v>183</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>134</v>
+    <row r="71" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>44</v>
@@ -4343,13 +4392,13 @@
         <v>180</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>139</v>
+        <v>76</v>
+      </c>
+      <c r="E71" s="7">
+        <v>1</v>
+      </c>
+      <c r="F71" s="7">
+        <v>1</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>109</v>
@@ -4357,146 +4406,140 @@
       <c r="H71" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I71" s="21" t="s">
+      <c r="I71" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="9">
+        <v>1</v>
+      </c>
+      <c r="F72" s="9">
+        <v>1</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I72" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I73" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="J71" s="7"/>
-    </row>
-    <row r="72" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C72" s="22" t="s">
+      <c r="B74" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D72" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72" s="23" t="s">
+      <c r="D74" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G72" s="22" t="s">
+      <c r="G74" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="H72" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I72" s="8" t="s">
+      <c r="H74" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I74" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-    </row>
-    <row r="73" spans="1:14" ht="150" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="G73" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I73" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-    </row>
-    <row r="74" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" s="22">
-        <v>1</v>
-      </c>
-      <c r="F74" s="22">
-        <v>1</v>
-      </c>
-      <c r="G74" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I74" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A75" s="22" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="D75" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="22">
-        <v>1</v>
-      </c>
-      <c r="F75" s="22">
-        <v>1</v>
+      <c r="E75" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="G75" s="22" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>44</v>
@@ -4520,22 +4563,22 @@
         <v>183</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="22" t="s">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="D77" s="22" t="s">
         <v>12</v>
@@ -4547,28 +4590,28 @@
         <v>1</v>
       </c>
       <c r="G77" s="22" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>223</v>
+        <v>270</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="22" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="D78" s="22" t="s">
         <v>12</v>
@@ -4580,88 +4623,88 @@
         <v>1</v>
       </c>
       <c r="G78" s="22" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:14" ht="180" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>144</v>
+    <row r="79" spans="1:14" ht="222" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="22" t="s">
+        <v>140</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="7">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7">
-        <v>1</v>
-      </c>
-      <c r="G79" s="7" t="s">
+      <c r="D79" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="22">
+        <v>1</v>
+      </c>
+      <c r="F79" s="22">
+        <v>1</v>
+      </c>
+      <c r="G79" s="22" t="s">
         <v>142</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>145</v>
+    <row r="80" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="7">
-        <v>1</v>
-      </c>
-      <c r="F80" s="7">
-        <v>6</v>
-      </c>
-      <c r="G80" s="7" t="s">
+      <c r="D80" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="22">
+        <v>1</v>
+      </c>
+      <c r="F80" s="22">
+        <v>1</v>
+      </c>
+      <c r="G80" s="22" t="s">
         <v>142</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>44</v>
@@ -4676,7 +4719,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>142</v>
@@ -4685,89 +4728,97 @@
         <v>183</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>217</v>
+        <v>283</v>
       </c>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+    <row r="82" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="7">
+        <v>1</v>
+      </c>
+      <c r="F82" s="7">
+        <v>6</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+    </row>
+    <row r="83" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="7">
+        <v>1</v>
+      </c>
+      <c r="F83" s="7">
+        <v>7</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+    </row>
+    <row r="84" spans="1:13" ht="250.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C82" s="8" t="s">
+      <c r="B84" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D82" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="22">
-        <v>1</v>
-      </c>
-      <c r="F82" s="22">
-        <v>1</v>
-      </c>
-      <c r="G82" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I82" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="219" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D83" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="22">
-        <v>1</v>
-      </c>
-      <c r="F83" s="22">
-        <v>1</v>
-      </c>
-      <c r="G83" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I83" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="255" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>243</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>17</v>
+      <c r="D84" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="22">
+        <v>1</v>
+      </c>
+      <c r="F84" s="22">
+        <v>1</v>
       </c>
       <c r="G84" s="22" t="s">
         <v>148</v>
@@ -4776,12 +4827,12 @@
         <v>183</v>
       </c>
       <c r="I84" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="219" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>44</v>
@@ -4796,7 +4847,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G85" s="22" t="s">
         <v>148</v>
@@ -4805,45 +4856,41 @@
         <v>183</v>
       </c>
       <c r="I85" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>151</v>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>243</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="2" t="s">
         <v>181</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="7">
-        <v>1</v>
-      </c>
-      <c r="F86" s="7">
-        <v>1</v>
-      </c>
-      <c r="G86" s="7" t="s">
+      <c r="E86" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G86" s="22" t="s">
         <v>148</v>
       </c>
       <c r="H86" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I86" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J86" s="7"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="7"/>
-      <c r="M86" s="7"/>
-    </row>
-    <row r="87" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>149</v>
+      <c r="I86" s="21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="204.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>44</v>
@@ -4851,35 +4898,31 @@
       <c r="C87" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G87" s="7" t="s">
+      <c r="D87" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="22">
+        <v>1</v>
+      </c>
+      <c r="F87" s="22">
+        <v>4</v>
+      </c>
+      <c r="G87" s="22" t="s">
         <v>148</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I87" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J87" s="7"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="7"/>
-      <c r="M87" s="7"/>
-    </row>
-    <row r="88" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>147</v>
+      <c r="I87" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>181</v>
@@ -4900,16 +4943,16 @@
         <v>183</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>284</v>
+        <v>152</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>44</v>
@@ -4917,31 +4960,35 @@
       <c r="C89" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D89" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="22">
-        <v>1</v>
-      </c>
-      <c r="F89" s="22">
-        <v>1</v>
-      </c>
-      <c r="G89" s="22" t="s">
+      <c r="D89" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G89" s="7" t="s">
         <v>148</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>183</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+    </row>
+    <row r="90" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>181</v>
@@ -4961,137 +5008,133 @@
       <c r="H90" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I90" s="21" t="s">
+      <c r="I90" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+    </row>
+    <row r="91" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="22">
+        <v>1</v>
+      </c>
+      <c r="F91" s="22">
+        <v>1</v>
+      </c>
+      <c r="G91" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I91" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="7">
+        <v>1</v>
+      </c>
+      <c r="F92" s="7">
+        <v>1</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I92" s="21" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+    <row r="93" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C91" s="8" t="s">
+      <c r="B93" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="7">
-        <v>1</v>
-      </c>
-      <c r="F91" s="7">
-        <v>1</v>
-      </c>
-      <c r="G91" s="7" t="s">
+      <c r="D93" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="7">
+        <v>1</v>
+      </c>
+      <c r="F93" s="7">
+        <v>1</v>
+      </c>
+      <c r="G93" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H91" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I91" s="8" t="s">
+      <c r="H93" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I93" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+    <row r="94" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C92" s="8" t="s">
+      <c r="B94" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="7">
-        <v>1</v>
-      </c>
-      <c r="F92" s="7">
-        <v>1</v>
-      </c>
-      <c r="G92" s="7" t="s">
+      <c r="D94" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="7">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1</v>
+      </c>
+      <c r="G94" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H92" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I92" s="8" t="s">
+      <c r="H94" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I94" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
+    <row r="95" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E93" s="7">
-        <v>1</v>
-      </c>
-      <c r="F93" s="7">
-        <v>1</v>
-      </c>
-      <c r="G93" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="7"/>
-      <c r="M93" s="7"/>
-    </row>
-    <row r="94" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" s="7">
-        <v>1</v>
-      </c>
-      <c r="F94" s="7">
-        <v>1</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I94" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-    </row>
-    <row r="95" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>44</v>
@@ -5115,16 +5158,16 @@
         <v>183</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>44</v>
@@ -5133,7 +5176,7 @@
         <v>162</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="E96" s="7">
         <v>1</v>
@@ -5148,161 +5191,169 @@
         <v>183</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E97" s="7">
+        <v>1</v>
+      </c>
+      <c r="F97" s="7">
+        <v>1</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="7"/>
+    </row>
+    <row r="98" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E98" s="7">
+        <v>1</v>
+      </c>
+      <c r="F98" s="7">
+        <v>1</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+      <c r="L98" s="7"/>
+      <c r="M98" s="7"/>
+    </row>
+    <row r="99" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C97" s="8" t="s">
+      <c r="B99" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E97" s="7">
-        <v>1</v>
-      </c>
-      <c r="F97" s="7">
-        <v>1</v>
-      </c>
-      <c r="G97" s="7" t="s">
+      <c r="D99" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="7">
+        <v>1</v>
+      </c>
+      <c r="F99" s="7">
+        <v>1</v>
+      </c>
+      <c r="G99" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H97" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I97" s="8" t="s">
+      <c r="H99" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I99" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C98" s="25" t="s">
+      <c r="B100" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F98" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G98" s="2" t="s">
+      <c r="D100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H98" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I98" s="24" t="s">
+      <c r="H100" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I100" s="24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="101" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>176</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C99" s="25" t="s">
+      <c r="B101" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C101" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E99" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G99" s="2" t="s">
+      <c r="D101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H99" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I99" s="24" t="s">
+      <c r="H101" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I101" s="24" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="102" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="30" t="s">
         <v>205</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E100" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I100" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>208</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F101" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="H101" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I101" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>210</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>44</v>
@@ -5326,70 +5377,70 @@
         <v>183</v>
       </c>
       <c r="I102" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H103" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I103" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I104" s="21" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="105" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H103" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="I103" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E104" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F104" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H104" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="I104" s="13" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>44</v>
@@ -5404,7 +5455,7 @@
         <v>13</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>231</v>
+        <v>33</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>228</v>
@@ -5412,13 +5463,13 @@
       <c r="H105" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="I105" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="I105" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>44</v>
@@ -5430,10 +5481,10 @@
         <v>12</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>228</v>
@@ -5441,71 +5492,71 @@
       <c r="H106" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="I106" s="15" t="s">
+      <c r="I106" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H107" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H108" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="I108" s="15" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="109" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C107" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="I107" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C108" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E108" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="H108" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="I108" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>44</v>
@@ -5528,70 +5579,128 @@
       <c r="H109" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="I109" s="5" t="s">
+      <c r="I109" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H110" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C111" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H111" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="I111" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="112" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>276</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C110" s="2" t="s">
+      <c r="B112" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D110" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F110" s="11" t="s">
+      <c r="D112" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F112" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H110" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I110" s="21" t="s">
+      <c r="H112" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I112" s="21" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="113" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>226</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C111" s="2" t="s">
+      <c r="B113" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F111" s="11" t="s">
+      <c r="D113" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F113" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H111" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I111" s="21" t="s">
+      <c r="H113" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I113" s="21" t="s">
         <v>275</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L111" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}"/>
+  <autoFilter ref="A1:L113" xr:uid="{E2A37AFA-B937-4BCB-B0F3-0C9B66FC5561}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -5601,13 +5710,13 @@
           <x14:formula1>
             <xm:f>lists!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D2</xm:sqref>
+          <xm:sqref>D1:D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DEE7F30C-7AF9-45DF-B494-649D45ADB1B7}">
           <x14:formula1>
             <xm:f>lists!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B111</xm:sqref>
+          <xm:sqref>B1:B113</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5623,12 +5732,12 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -5636,7 +5745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5644,7 +5753,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>171</v>
       </c>

</xml_diff>